<commit_message>
adjustments before review submission
</commit_message>
<xml_diff>
--- a/results/FrequencyTables/26775808_sgRNA-8.xlsx
+++ b/results/FrequencyTables/26775808_sgRNA-8.xlsx
@@ -465,73 +465,73 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.239322533136966</v>
+        <v>0.119259259259259</v>
       </c>
       <c r="C2">
-        <v>0.0331369661266568</v>
+        <v>0.0407407407407407</v>
       </c>
       <c r="D2">
-        <v>0.0147275405007364</v>
+        <v>0.0155555555555556</v>
       </c>
       <c r="E2">
-        <v>0.00368188512518409</v>
+        <v>0.00592592592592593</v>
       </c>
       <c r="F2">
-        <v>0.166421207658321</v>
+        <v>0.02</v>
       </c>
       <c r="G2">
-        <v>0.00294550810014728</v>
+        <v>0.0103703703703704</v>
       </c>
       <c r="H2">
-        <v>0.000736377025036819</v>
+        <v>0.00444444444444444</v>
       </c>
       <c r="I2">
-        <v>0.00662739322533137</v>
+        <v>0.00444444444444444</v>
       </c>
       <c r="J2">
-        <v>0.0176730486008837</v>
+        <v>0.017037037037037</v>
       </c>
       <c r="K2">
-        <v>0.00441826215022091</v>
+        <v>0.00222222222222222</v>
       </c>
       <c r="L2">
-        <v>0.00957290132547865</v>
+        <v>0.0111111111111111</v>
       </c>
       <c r="M2">
-        <v>0.846833578792342</v>
+        <v>0.979259259259259</v>
       </c>
       <c r="N2">
-        <v>0.00515463917525773</v>
+        <v>0.00592592592592593</v>
       </c>
       <c r="O2">
-        <v>0.00957290132547865</v>
+        <v>0.0407407407407407</v>
       </c>
       <c r="P2">
-        <v>0.0191458026509573</v>
+        <v>0.0244444444444444</v>
       </c>
       <c r="Q2">
-        <v>0.00368188512518409</v>
+        <v>0.00666666666666667</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>0.00222222222222222</v>
       </c>
       <c r="S2">
-        <v>0.00441826215022091</v>
+        <v>0.0037037037037037</v>
       </c>
       <c r="T2">
-        <v>0.993372606774669</v>
+        <v>0.995555555555556</v>
       </c>
       <c r="U2">
-        <v>0.0103092783505155</v>
+        <v>0.00592592592592593</v>
       </c>
       <c r="V2">
-        <v>0.00368188512518409</v>
+        <v>0.00148148148148148</v>
       </c>
       <c r="W2">
-        <v>0.00957290132547865</v>
+        <v>0.00888888888888889</v>
       </c>
       <c r="X2">
-        <v>0.00220913107511046</v>
+        <v>0.000740740740740741</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -539,55 +539,55 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.0184094256259205</v>
+        <v>0.0177777777777778</v>
       </c>
       <c r="C3">
-        <v>0.770986745213549</v>
+        <v>0.900740740740741</v>
       </c>
       <c r="D3">
-        <v>0.818851251840943</v>
+        <v>0.951111111111111</v>
       </c>
       <c r="E3">
-        <v>0.00441826215022091</v>
+        <v>0.000740740740740741</v>
       </c>
       <c r="F3">
-        <v>0.00736377025036819</v>
+        <v>0.00666666666666667</v>
       </c>
       <c r="G3">
-        <v>0.164948453608247</v>
+        <v>0.0185185185185185</v>
       </c>
       <c r="H3">
-        <v>0.00515463917525773</v>
+        <v>0.0111111111111111</v>
       </c>
       <c r="I3">
-        <v>0.815905743740795</v>
+        <v>0.952592592592593</v>
       </c>
       <c r="J3">
-        <v>0.00736377025036819</v>
+        <v>0.00666666666666667</v>
       </c>
       <c r="K3">
-        <v>0.156848306332842</v>
+        <v>0.00666666666666667</v>
       </c>
       <c r="L3">
-        <v>0.156111929307806</v>
+        <v>0.00740740740740741</v>
       </c>
       <c r="M3">
-        <v>0.00147275405007364</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>0.981590574374079</v>
+        <v>0.964444444444444</v>
       </c>
       <c r="O3">
-        <v>0.00441826215022091</v>
+        <v>0.0851851851851852</v>
       </c>
       <c r="P3">
-        <v>0.000736377025036819</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>0.00220913107511046</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>0.00810014727540501</v>
+        <v>0.0222222222222222</v>
       </c>
       <c r="S3">
         <v>0</v>
@@ -596,16 +596,16 @@
         <v>0</v>
       </c>
       <c r="U3">
-        <v>0.1620029455081</v>
+        <v>0.00666666666666667</v>
       </c>
       <c r="V3">
-        <v>0.0125184094256259</v>
+        <v>0.0244444444444444</v>
       </c>
       <c r="W3">
-        <v>0.0147275405007364</v>
+        <v>0.0266666666666667</v>
       </c>
       <c r="X3">
-        <v>0.0139911634756996</v>
+        <v>0.0251851851851852</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -613,73 +613,73 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.733431516936672</v>
+        <v>0.855555555555556</v>
       </c>
       <c r="C4">
-        <v>0.163475699558174</v>
+        <v>0.0214814814814815</v>
       </c>
       <c r="D4">
-        <v>0.1620029455081</v>
+        <v>0.0266666666666667</v>
       </c>
       <c r="E4">
-        <v>0.181885125184094</v>
+        <v>0.0466666666666667</v>
       </c>
       <c r="F4">
-        <v>0.823269513991163</v>
+        <v>0.971851851851852</v>
       </c>
       <c r="G4">
-        <v>0.822533136966127</v>
+        <v>0.964444444444444</v>
       </c>
       <c r="H4">
-        <v>0.835051546391753</v>
+        <v>0.975555555555556</v>
       </c>
       <c r="I4">
-        <v>0.0103092783505155</v>
+        <v>0.0155555555555556</v>
       </c>
       <c r="J4">
-        <v>0.815905743740795</v>
+        <v>0.967407407407407</v>
       </c>
       <c r="K4">
-        <v>0.831369661266569</v>
+        <v>0.985925925925926</v>
       </c>
       <c r="L4">
-        <v>0.832106038291605</v>
+        <v>0.980740740740741</v>
       </c>
       <c r="M4">
-        <v>0.150220913107511</v>
+        <v>0.0192592592592593</v>
       </c>
       <c r="N4">
-        <v>0.00589101620029455</v>
+        <v>0.0207407407407407</v>
       </c>
       <c r="O4">
-        <v>0.000736377025036819</v>
+        <v>0.0192592592592593</v>
       </c>
       <c r="P4">
-        <v>0.980117820324006</v>
+        <v>0.974074074074074</v>
       </c>
       <c r="Q4">
-        <v>0.993372606774669</v>
+        <v>0.993333333333333</v>
       </c>
       <c r="R4">
-        <v>0.988954344624448</v>
+        <v>0.974814814814815</v>
       </c>
       <c r="S4">
-        <v>0.995581737849779</v>
+        <v>0.995555555555556</v>
       </c>
       <c r="T4">
-        <v>0.00368188512518409</v>
+        <v>0.00222222222222222</v>
       </c>
       <c r="U4">
-        <v>0.826951399116348</v>
+        <v>0.986666666666667</v>
       </c>
       <c r="V4">
-        <v>0.0235640648011782</v>
+        <v>0.0222222222222222</v>
       </c>
       <c r="W4">
-        <v>0.814432989690722</v>
+        <v>0.956296296296296</v>
       </c>
       <c r="X4">
-        <v>0.824742268041237</v>
+        <v>0.965185185185185</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -687,73 +687,73 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.00810014727540501</v>
+        <v>0.00666666666666667</v>
       </c>
       <c r="C5">
-        <v>0.0309278350515464</v>
+        <v>0.0362962962962963</v>
       </c>
       <c r="D5">
-        <v>0.00441826215022091</v>
+        <v>0.00666666666666667</v>
       </c>
       <c r="E5">
-        <v>0.810014727540501</v>
+        <v>0.946666666666667</v>
       </c>
       <c r="F5">
-        <v>0.00294550810014728</v>
+        <v>0.000740740740740741</v>
       </c>
       <c r="G5">
-        <v>0.00957290132547865</v>
+        <v>0.00666666666666667</v>
       </c>
       <c r="H5">
-        <v>0.157584683357879</v>
+        <v>0.00740740740740741</v>
       </c>
       <c r="I5">
-        <v>0.167157584683358</v>
+        <v>0.0274074074074074</v>
       </c>
       <c r="J5">
-        <v>0.159057437407953</v>
+        <v>0.00814814814814815</v>
       </c>
       <c r="K5">
-        <v>0.00736377025036819</v>
+        <v>0.00518518518518519</v>
       </c>
       <c r="L5">
-        <v>0.00220913107511046</v>
+        <v>0.000740740740740741</v>
       </c>
       <c r="M5">
-        <v>0.00147275405007364</v>
+        <v>0.00148148148148148</v>
       </c>
       <c r="N5">
-        <v>0.00736377025036819</v>
+        <v>0.00888888888888889</v>
       </c>
       <c r="O5">
-        <v>0.985272459499264</v>
+        <v>0.854814814814815</v>
       </c>
       <c r="P5">
+        <v>0.00148148148148148</v>
+      </c>
+      <c r="Q5">
         <v>0</v>
       </c>
-      <c r="Q5">
-        <v>0.000736377025036819</v>
-      </c>
       <c r="R5">
-        <v>0.00294550810014728</v>
+        <v>0.000740740740740741</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>0.000740740740740741</v>
       </c>
       <c r="T5">
-        <v>0.00294550810014728</v>
+        <v>0.00222222222222222</v>
       </c>
       <c r="U5">
-        <v>0.000736377025036819</v>
+        <v>0.000740740740740741</v>
       </c>
       <c r="V5">
-        <v>0.960235640648012</v>
+        <v>0.951851851851852</v>
       </c>
       <c r="W5">
-        <v>0.161266568483063</v>
+        <v>0.00814814814814815</v>
       </c>
       <c r="X5">
-        <v>0.158321060382916</v>
+        <v>0.00814814814814815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>